<commit_message>
18 May 2025 update
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/embedded.xlsx
+++ b/xlsxPCES/examples/embedded.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesapps/embedded/xlsx/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld/xlsxPCES/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB9C8BA-6EFA-D043-917B-6672225C9CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4379B6-9954-3947-A706-224B7B310D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1220" windowWidth="34560" windowHeight="20160" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="3860" yWindow="840" windowWidth="34560" windowHeight="20160" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="206">
   <si>
     <t>Networks</t>
   </si>
@@ -566,18 +566,6 @@
   </si>
   <si>
     <t>$bndwdth,netParams</t>
-  </si>
-  <si>
-    <t>exp-5</t>
-  </si>
-  <si>
-    <t>exp-6</t>
-  </si>
-  <si>
-    <t>exp-7</t>
-  </si>
-  <si>
-    <t>exp-8</t>
   </si>
   <si>
     <t>AMD EPYC 7763 64-Core Processor</t>
@@ -1250,7 +1238,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1272,8 +1260,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1751,7 +1738,7 @@
         <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
@@ -1835,7 +1822,7 @@
         <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" s="7">
         <v>1</v>
@@ -1859,7 +1846,7 @@
         <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
@@ -1879,7 +1866,7 @@
         <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C21" s="7">
         <v>1</v>
@@ -1953,7 +1940,7 @@
         <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>24</v>
@@ -1991,7 +1978,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA9935-1338-5743-9994-8B53C9940146}">
-  <dimension ref="A3:N100"/>
+  <dimension ref="A3:M100"/>
   <sheetViews>
     <sheetView topLeftCell="E42" zoomScale="155" zoomScaleNormal="164" workbookViewId="0">
       <selection activeCell="L45" sqref="L45"/>
@@ -2441,12 +2428,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>83</v>
       </c>
@@ -2486,9 +2473,8 @@
       <c r="M52" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N52" s="15"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -2508,7 +2494,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -2528,7 +2514,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>73</v>
       </c>
@@ -2551,10 +2537,10 @@
         <v>112</v>
       </c>
       <c r="I55" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -2577,10 +2563,10 @@
         <v>112</v>
       </c>
       <c r="I56" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>84</v>
       </c>
@@ -2612,7 +2598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>75</v>
       </c>
@@ -2635,7 +2621,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>75</v>
       </c>
@@ -2658,7 +2644,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -2672,7 +2658,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F64" t="s">
         <v>117</v>
       </c>
@@ -2954,7 +2940,7 @@
         <v>20</v>
       </c>
       <c r="E82" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F82" t="b">
         <v>1</v>
@@ -2977,7 +2963,7 @@
         <v>117</v>
       </c>
       <c r="E84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F84" t="b">
         <v>1</v>
@@ -3120,15 +3106,15 @@
         <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
         <v>115</v>
@@ -3142,7 +3128,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
         <v>115</v>
@@ -3156,7 +3142,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>127</v>
@@ -3170,7 +3156,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
         <v>127</v>
@@ -3184,7 +3170,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
         <v>127</v>
@@ -3198,7 +3184,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
         <v>127</v>
@@ -3212,7 +3198,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
         <v>127</v>
@@ -3226,7 +3212,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>127</v>
@@ -3240,7 +3226,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
         <v>127</v>
@@ -3254,7 +3240,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B12" t="s">
         <v>127</v>
@@ -3268,7 +3254,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
         <v>127</v>
@@ -3282,10 +3268,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C14">
         <v>64</v>
@@ -3296,10 +3282,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C15">
         <v>128</v>
@@ -3310,10 +3296,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C16">
         <v>196</v>
@@ -3324,10 +3310,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C17">
         <v>256</v>
@@ -3338,10 +3324,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C18">
         <v>384</v>
@@ -3352,10 +3338,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C19">
         <v>512</v>
@@ -3366,10 +3352,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C20">
         <v>768</v>
@@ -3380,10 +3366,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C21">
         <v>1000</v>
@@ -3394,10 +3380,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C22">
         <v>1500</v>
@@ -3408,10 +3394,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C23">
         <v>64</v>
@@ -3422,10 +3408,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C24">
         <v>128</v>
@@ -3436,10 +3422,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C25">
         <v>196</v>
@@ -3450,10 +3436,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C26">
         <v>256</v>
@@ -3464,10 +3450,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C27">
         <v>384</v>
@@ -3478,10 +3464,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C28">
         <v>512</v>
@@ -3492,10 +3478,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C29">
         <v>768</v>
@@ -3506,10 +3492,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C30">
         <v>1000</v>
@@ -3520,10 +3506,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C31">
         <v>1500</v>
@@ -3534,10 +3520,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B32" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C32">
         <v>64</v>
@@ -3548,10 +3534,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C33">
         <v>128</v>
@@ -3562,10 +3548,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C34">
         <v>196</v>
@@ -3576,10 +3562,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B35" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C35">
         <v>256</v>
@@ -3590,10 +3576,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B36" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C36">
         <v>384</v>
@@ -3604,10 +3590,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C37">
         <v>512</v>
@@ -3618,10 +3604,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B38" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C38">
         <v>768</v>
@@ -3632,10 +3618,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C39">
         <v>1000</v>
@@ -3646,10 +3632,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C40">
         <v>1500</v>
@@ -3660,7 +3646,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B41" t="s">
         <v>124</v>
@@ -3674,7 +3660,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>124</v>
@@ -3688,7 +3674,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B43" t="s">
         <v>124</v>
@@ -3702,7 +3688,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B44" t="s">
         <v>124</v>
@@ -3716,7 +3702,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B45" t="s">
         <v>124</v>
@@ -3730,7 +3716,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B46" t="s">
         <v>124</v>
@@ -3744,7 +3730,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
         <v>124</v>
@@ -3758,7 +3744,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
         <v>124</v>
@@ -3772,7 +3758,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
         <v>124</v>
@@ -3786,10 +3772,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" t="s">
         <v>180</v>
-      </c>
-      <c r="B50" t="s">
-        <v>184</v>
       </c>
       <c r="C50">
         <v>64</v>
@@ -3800,10 +3786,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B51" t="s">
         <v>180</v>
-      </c>
-      <c r="B51" t="s">
-        <v>184</v>
       </c>
       <c r="C51">
         <v>128</v>
@@ -3814,10 +3800,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
         <v>180</v>
-      </c>
-      <c r="B52" t="s">
-        <v>184</v>
       </c>
       <c r="C52">
         <v>196</v>
@@ -3828,10 +3814,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>176</v>
+      </c>
+      <c r="B53" t="s">
         <v>180</v>
-      </c>
-      <c r="B53" t="s">
-        <v>184</v>
       </c>
       <c r="C53">
         <v>256</v>
@@ -3842,10 +3828,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>176</v>
+      </c>
+      <c r="B54" t="s">
         <v>180</v>
-      </c>
-      <c r="B54" t="s">
-        <v>184</v>
       </c>
       <c r="C54">
         <v>384</v>
@@ -3856,10 +3842,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>176</v>
+      </c>
+      <c r="B55" t="s">
         <v>180</v>
-      </c>
-      <c r="B55" t="s">
-        <v>184</v>
       </c>
       <c r="C55">
         <v>512</v>
@@ -3870,10 +3856,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
         <v>180</v>
-      </c>
-      <c r="B56" t="s">
-        <v>184</v>
       </c>
       <c r="C56">
         <v>768</v>
@@ -3884,10 +3870,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" t="s">
         <v>180</v>
-      </c>
-      <c r="B57" t="s">
-        <v>184</v>
       </c>
       <c r="C57">
         <v>1000</v>
@@ -3898,10 +3884,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" t="s">
         <v>180</v>
-      </c>
-      <c r="B58" t="s">
-        <v>184</v>
       </c>
       <c r="C58">
         <v>1500</v>
@@ -3912,10 +3898,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B59" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C59">
         <v>64</v>
@@ -3926,10 +3912,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C60">
         <v>128</v>
@@ -3940,10 +3926,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C61">
         <v>196</v>
@@ -3954,10 +3940,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C62">
         <v>256</v>
@@ -3968,10 +3954,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B63" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C63">
         <v>384</v>
@@ -3982,10 +3968,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C64">
         <v>512</v>
@@ -3996,10 +3982,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C65">
         <v>768</v>
@@ -4010,10 +3996,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C66">
         <v>1000</v>
@@ -4024,10 +4010,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B67" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C67">
         <v>1500</v>
@@ -4038,10 +4024,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B68" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C68">
         <v>64</v>
@@ -4052,10 +4038,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C69">
         <v>128</v>
@@ -4066,10 +4052,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C70">
         <v>196</v>
@@ -4080,10 +4066,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C71">
         <v>256</v>
@@ -4094,10 +4080,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C72">
         <v>384</v>
@@ -4108,10 +4094,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B73" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C73">
         <v>512</v>
@@ -4122,10 +4108,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B74" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C74">
         <v>768</v>
@@ -4136,10 +4122,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C75">
         <v>1000</v>
@@ -4150,10 +4136,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B76" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C76">
         <v>1500</v>
@@ -4164,7 +4150,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B77" t="s">
         <v>126</v>
@@ -4178,7 +4164,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B78" t="s">
         <v>126</v>
@@ -4192,7 +4178,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B79" t="s">
         <v>126</v>
@@ -4206,7 +4192,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B80" t="s">
         <v>126</v>
@@ -4220,7 +4206,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B81" t="s">
         <v>126</v>
@@ -4234,7 +4220,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
         <v>126</v>
@@ -4248,7 +4234,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
         <v>126</v>
@@ -4262,7 +4248,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
         <v>126</v>
@@ -4276,7 +4262,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B85" t="s">
         <v>126</v>
@@ -4290,10 +4276,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C86">
         <v>64</v>
@@ -4304,10 +4290,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C87">
         <v>128</v>
@@ -4318,10 +4304,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C88">
         <v>196</v>
@@ -4332,10 +4318,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C89">
         <v>256</v>
@@ -4346,10 +4332,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C90">
         <v>384</v>
@@ -4360,10 +4346,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C91">
         <v>512</v>
@@ -4374,10 +4360,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C92">
         <v>768</v>
@@ -4388,10 +4374,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C93">
         <v>1000</v>
@@ -4402,10 +4388,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B94" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C94">
         <v>1500</v>
@@ -4416,10 +4402,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C95">
         <v>64</v>
@@ -4430,10 +4416,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C96">
         <v>128</v>
@@ -4444,10 +4430,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C97">
         <v>196</v>
@@ -4458,10 +4444,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C98">
         <v>256</v>
@@ -4472,10 +4458,10 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C99">
         <v>384</v>
@@ -4486,10 +4472,10 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C100">
         <v>512</v>
@@ -4500,10 +4486,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C101">
         <v>768</v>
@@ -4514,10 +4500,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B102" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C102">
         <v>1000</v>
@@ -4528,10 +4514,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C103">
         <v>1500</v>
@@ -4542,10 +4528,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C104">
         <v>64</v>
@@ -4556,10 +4542,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B105" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C105">
         <v>128</v>
@@ -4570,10 +4556,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C106">
         <v>196</v>
@@ -4584,10 +4570,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C107">
         <v>256</v>
@@ -4598,10 +4584,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C108">
         <v>384</v>
@@ -4612,10 +4598,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C109">
         <v>512</v>
@@ -4626,10 +4612,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C110">
         <v>768</v>
@@ -4640,10 +4626,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C111">
         <v>1000</v>
@@ -4654,10 +4640,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B112" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C112">
         <v>1500</v>
@@ -4668,7 +4654,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B113" t="s">
         <v>123</v>
@@ -4682,7 +4668,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B114" t="s">
         <v>123</v>
@@ -4696,7 +4682,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B115" t="s">
         <v>123</v>
@@ -4710,7 +4696,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B116" t="s">
         <v>123</v>
@@ -4724,7 +4710,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B117" t="s">
         <v>123</v>
@@ -4738,7 +4724,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B118" t="s">
         <v>123</v>
@@ -4752,7 +4738,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B119" t="s">
         <v>123</v>
@@ -4766,7 +4752,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B120" t="s">
         <v>123</v>
@@ -4780,7 +4766,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B121" t="s">
         <v>123</v>
@@ -4794,10 +4780,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C122">
         <v>64</v>
@@ -4808,10 +4794,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B123" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C123">
         <v>128</v>
@@ -4822,10 +4808,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B124" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C124">
         <v>196</v>
@@ -4836,10 +4822,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B125" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C125">
         <v>256</v>
@@ -4850,10 +4836,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C126">
         <v>384</v>
@@ -4864,10 +4850,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B127" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C127">
         <v>512</v>
@@ -4878,10 +4864,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B128" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C128">
         <v>768</v>
@@ -4892,10 +4878,10 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B129" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C129">
         <v>1000</v>
@@ -4906,10 +4892,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B130" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C130">
         <v>1500</v>
@@ -4920,10 +4906,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C131">
         <v>64</v>
@@ -4934,10 +4920,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B132" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C132">
         <v>128</v>
@@ -4948,10 +4934,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B133" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C133">
         <v>196</v>
@@ -4962,10 +4948,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B134" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C134">
         <v>256</v>
@@ -4976,10 +4962,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B135" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C135">
         <v>384</v>
@@ -4990,10 +4976,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B136" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C136">
         <v>512</v>
@@ -5004,10 +4990,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B137" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C137">
         <v>768</v>
@@ -5018,10 +5004,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B138" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C138">
         <v>1000</v>
@@ -5032,10 +5018,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B139" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C139">
         <v>1500</v>
@@ -5046,10 +5032,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B140" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C140">
         <v>64</v>
@@ -5060,10 +5046,10 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B141" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C141">
         <v>128</v>
@@ -5074,10 +5060,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B142" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C142">
         <v>196</v>
@@ -5088,10 +5074,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B143" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C143">
         <v>256</v>
@@ -5102,10 +5088,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B144" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C144">
         <v>384</v>
@@ -5116,10 +5102,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B145" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C145">
         <v>512</v>
@@ -5130,10 +5116,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B146" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C146">
         <v>768</v>
@@ -5144,10 +5130,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B147" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C147">
         <v>1000</v>
@@ -5158,10 +5144,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B148" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C148">
         <v>1500</v>
@@ -5172,7 +5158,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B149" t="s">
         <v>125</v>
@@ -5186,7 +5172,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B150" t="s">
         <v>125</v>
@@ -5200,7 +5186,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B151" t="s">
         <v>125</v>
@@ -5214,7 +5200,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B152" t="s">
         <v>125</v>
@@ -5228,7 +5214,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B153" t="s">
         <v>125</v>
@@ -5242,7 +5228,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B154" t="s">
         <v>125</v>
@@ -5256,7 +5242,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B155" t="s">
         <v>125</v>
@@ -5270,7 +5256,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B156" t="s">
         <v>125</v>
@@ -5284,7 +5270,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B157" t="s">
         <v>125</v>
@@ -5298,7 +5284,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B158" t="s">
         <v>127</v>
@@ -5312,7 +5298,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B159" t="s">
         <v>127</v>
@@ -5326,7 +5312,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B160" t="s">
         <v>127</v>
@@ -5340,7 +5326,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B161" t="s">
         <v>127</v>
@@ -5354,7 +5340,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B162" t="s">
         <v>127</v>
@@ -5368,7 +5354,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B163" t="s">
         <v>127</v>
@@ -5382,7 +5368,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B164" t="s">
         <v>127</v>
@@ -5396,7 +5382,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B165" t="s">
         <v>127</v>
@@ -5410,7 +5396,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B166" t="s">
         <v>127</v>
@@ -5424,10 +5410,10 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B167" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C167">
         <v>64</v>
@@ -5438,10 +5424,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B168" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C168">
         <v>128</v>
@@ -5452,10 +5438,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B169" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C169">
         <v>196</v>
@@ -5466,10 +5452,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B170" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C170">
         <v>256</v>
@@ -5480,10 +5466,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B171" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C171">
         <v>384</v>
@@ -5494,10 +5480,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B172" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C172">
         <v>512</v>
@@ -5508,10 +5494,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B173" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C173">
         <v>768</v>
@@ -5522,10 +5508,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B174" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C174">
         <v>1000</v>
@@ -5536,10 +5522,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B175" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C175">
         <v>1500</v>
@@ -5550,10 +5536,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C176">
         <v>64</v>
@@ -5564,10 +5550,10 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B177" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C177">
         <v>128</v>
@@ -5578,10 +5564,10 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B178" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C178">
         <v>196</v>
@@ -5592,10 +5578,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B179" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C179">
         <v>256</v>
@@ -5606,10 +5592,10 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B180" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C180">
         <v>384</v>
@@ -5620,10 +5606,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B181" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C181">
         <v>512</v>
@@ -5634,10 +5620,10 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B182" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C182">
         <v>768</v>
@@ -5648,10 +5634,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B183" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C183">
         <v>1000</v>
@@ -5662,10 +5648,10 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B184" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C184">
         <v>1500</v>
@@ -5676,10 +5662,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B185" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C185">
         <v>64</v>
@@ -5690,10 +5676,10 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B186" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C186">
         <v>128</v>
@@ -5704,10 +5690,10 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B187" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C187">
         <v>196</v>
@@ -5718,10 +5704,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B188" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C188">
         <v>256</v>
@@ -5732,10 +5718,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B189" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C189">
         <v>384</v>
@@ -5746,10 +5732,10 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C190">
         <v>512</v>
@@ -5760,10 +5746,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C191">
         <v>768</v>
@@ -5774,10 +5760,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B192" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C192">
         <v>1000</v>
@@ -5788,10 +5774,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B193" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C193">
         <v>1500</v>
@@ -5802,7 +5788,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B194" t="s">
         <v>124</v>
@@ -5816,7 +5802,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B195" t="s">
         <v>124</v>
@@ -5830,7 +5816,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B196" t="s">
         <v>124</v>
@@ -5844,7 +5830,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B197" t="s">
         <v>124</v>
@@ -5858,7 +5844,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B198" t="s">
         <v>124</v>
@@ -5872,7 +5858,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B199" t="s">
         <v>124</v>
@@ -5886,7 +5872,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B200" t="s">
         <v>124</v>
@@ -5900,7 +5886,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B201" t="s">
         <v>124</v>
@@ -5914,7 +5900,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B202" t="s">
         <v>124</v>
@@ -5928,10 +5914,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B203" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C203">
         <v>64</v>
@@ -5942,10 +5928,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B204" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C204">
         <v>128</v>
@@ -5956,10 +5942,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B205" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C205">
         <v>196</v>
@@ -5970,10 +5956,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B206" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C206">
         <v>256</v>
@@ -5984,10 +5970,10 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B207" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C207">
         <v>384</v>
@@ -5998,10 +5984,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B208" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C208">
         <v>512</v>
@@ -6012,10 +5998,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B209" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C209">
         <v>768</v>
@@ -6026,10 +6012,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B210" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C210">
         <v>1000</v>
@@ -6040,10 +6026,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B211" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C211">
         <v>1500</v>
@@ -6054,10 +6040,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B212" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C212">
         <v>64</v>
@@ -6068,10 +6054,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B213" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C213">
         <v>128</v>
@@ -6082,10 +6068,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B214" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C214">
         <v>196</v>
@@ -6096,10 +6082,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B215" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C215">
         <v>256</v>
@@ -6110,10 +6096,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B216" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C216">
         <v>384</v>
@@ -6124,10 +6110,10 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B217" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C217">
         <v>512</v>
@@ -6138,10 +6124,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B218" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C218">
         <v>768</v>
@@ -6152,10 +6138,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B219" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C219">
         <v>1000</v>
@@ -6166,10 +6152,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B220" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C220">
         <v>1500</v>
@@ -6180,10 +6166,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B221" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C221">
         <v>64</v>
@@ -6194,10 +6180,10 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B222" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C222">
         <v>128</v>
@@ -6208,10 +6194,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B223" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C223">
         <v>196</v>
@@ -6222,10 +6208,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B224" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C224">
         <v>256</v>
@@ -6236,10 +6222,10 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B225" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C225">
         <v>384</v>
@@ -6250,10 +6236,10 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B226" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C226">
         <v>512</v>
@@ -6264,10 +6250,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B227" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C227">
         <v>768</v>
@@ -6278,10 +6264,10 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B228" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C228">
         <v>1000</v>
@@ -6292,10 +6278,10 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B229" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C229">
         <v>1500</v>
@@ -6306,10 +6292,10 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B230" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C230">
         <v>64</v>
@@ -6320,10 +6306,10 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B231" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C231">
         <v>128</v>
@@ -6334,10 +6320,10 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B232" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C232">
         <v>196</v>
@@ -6348,10 +6334,10 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B233" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C233">
         <v>64</v>
@@ -6362,10 +6348,10 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B234" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C234">
         <v>128</v>
@@ -6376,10 +6362,10 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B235" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C235">
         <v>196</v>
@@ -6390,10 +6376,10 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B236" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C236">
         <v>256</v>
@@ -6404,7 +6390,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B237" t="s">
         <v>126</v>
@@ -6418,7 +6404,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B238" t="s">
         <v>126</v>
@@ -6432,7 +6418,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B239" t="s">
         <v>126</v>
@@ -6446,7 +6432,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B240" t="s">
         <v>126</v>
@@ -6460,7 +6446,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B241" t="s">
         <v>126</v>
@@ -6474,7 +6460,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B242" t="s">
         <v>126</v>
@@ -6488,7 +6474,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B243" t="s">
         <v>126</v>
@@ -6502,7 +6488,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B244" t="s">
         <v>126</v>
@@ -6516,7 +6502,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B245" t="s">
         <v>126</v>
@@ -6530,10 +6516,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B246" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C246">
         <v>64</v>
@@ -6544,10 +6530,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B247" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C247">
         <v>128</v>
@@ -6558,10 +6544,10 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B248" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C248">
         <v>196</v>
@@ -6572,10 +6558,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B249" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C249">
         <v>256</v>
@@ -6586,10 +6572,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B250" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C250">
         <v>384</v>
@@ -6600,10 +6586,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B251" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C251">
         <v>512</v>
@@ -6614,10 +6600,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B252" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C252">
         <v>768</v>
@@ -6628,10 +6614,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B253" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C253">
         <v>1000</v>
@@ -6642,10 +6628,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B254" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C254">
         <v>1500</v>
@@ -6656,10 +6642,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B255" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C255">
         <v>64</v>
@@ -6670,10 +6656,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B256" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C256">
         <v>128</v>
@@ -6684,10 +6670,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B257" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C257">
         <v>196</v>
@@ -6698,10 +6684,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B258" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C258">
         <v>256</v>
@@ -6712,10 +6698,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B259" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C259">
         <v>384</v>
@@ -6726,10 +6712,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B260" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C260">
         <v>512</v>
@@ -6740,10 +6726,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B261" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C261">
         <v>768</v>
@@ -6754,10 +6740,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B262" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C262">
         <v>1000</v>
@@ -6768,10 +6754,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B263" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C263">
         <v>1500</v>
@@ -6782,10 +6768,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B264" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C264">
         <v>64</v>
@@ -6796,10 +6782,10 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B265" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C265">
         <v>128</v>
@@ -6810,10 +6796,10 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B266" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C266">
         <v>196</v>
@@ -6824,10 +6810,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B267" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C267">
         <v>256</v>
@@ -6838,10 +6824,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B268" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C268">
         <v>384</v>
@@ -6852,10 +6838,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B269" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C269">
         <v>512</v>
@@ -6866,10 +6852,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B270" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C270">
         <v>768</v>
@@ -6880,10 +6866,10 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B271" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C271">
         <v>1000</v>
@@ -6894,10 +6880,10 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B272" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C272">
         <v>1500</v>
@@ -6908,7 +6894,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B273" t="s">
         <v>123</v>
@@ -6922,7 +6908,7 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B274" t="s">
         <v>123</v>
@@ -6936,7 +6922,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B275" t="s">
         <v>123</v>
@@ -6950,7 +6936,7 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B276" t="s">
         <v>123</v>
@@ -6964,7 +6950,7 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B277" t="s">
         <v>123</v>
@@ -6978,7 +6964,7 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B278" t="s">
         <v>123</v>
@@ -6992,7 +6978,7 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B279" t="s">
         <v>123</v>
@@ -7006,7 +6992,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B280" t="s">
         <v>123</v>
@@ -7020,7 +7006,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B281" t="s">
         <v>123</v>
@@ -7034,10 +7020,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B282" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C282">
         <v>64</v>
@@ -7048,10 +7034,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B283" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C283">
         <v>128</v>
@@ -7062,10 +7048,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B284" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C284">
         <v>196</v>
@@ -7076,10 +7062,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B285" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C285">
         <v>256</v>
@@ -7090,10 +7076,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B286" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C286">
         <v>384</v>
@@ -7104,10 +7090,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B287" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C287">
         <v>512</v>
@@ -7118,10 +7104,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B288" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C288">
         <v>768</v>
@@ -7132,10 +7118,10 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B289" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C289">
         <v>1000</v>
@@ -7146,10 +7132,10 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B290" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C290">
         <v>1500</v>
@@ -7160,10 +7146,10 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B291" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C291">
         <v>64</v>
@@ -7174,10 +7160,10 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B292" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C292">
         <v>128</v>
@@ -7188,10 +7174,10 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B293" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C293">
         <v>196</v>
@@ -7202,10 +7188,10 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B294" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C294">
         <v>256</v>
@@ -7216,10 +7202,10 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B295" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C295">
         <v>384</v>
@@ -7230,10 +7216,10 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B296" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C296">
         <v>512</v>
@@ -7244,10 +7230,10 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B297" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C297">
         <v>768</v>
@@ -7258,10 +7244,10 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B298" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C298">
         <v>1000</v>
@@ -7272,10 +7258,10 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B299" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C299">
         <v>1500</v>
@@ -7286,10 +7272,10 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B300" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C300">
         <v>64</v>
@@ -7300,10 +7286,10 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B301" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C301">
         <v>128</v>
@@ -7314,10 +7300,10 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B302" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C302">
         <v>196</v>
@@ -7328,10 +7314,10 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B303" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C303">
         <v>256</v>
@@ -7342,10 +7328,10 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B304" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C304">
         <v>384</v>
@@ -7356,10 +7342,10 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B305" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C305">
         <v>512</v>
@@ -7370,10 +7356,10 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B306" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C306">
         <v>768</v>
@@ -7384,10 +7370,10 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B307" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C307">
         <v>1000</v>
@@ -7398,10 +7384,10 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B308" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C308">
         <v>1500</v>
@@ -7412,10 +7398,10 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B309" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C309">
         <v>64</v>
@@ -7426,10 +7412,10 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B310" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C310">
         <v>128</v>
@@ -7440,10 +7426,10 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B311" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C311">
         <v>196</v>
@@ -7454,10 +7440,10 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
+        <v>189</v>
+      </c>
+      <c r="B312" t="s">
         <v>193</v>
-      </c>
-      <c r="B312" t="s">
-        <v>197</v>
       </c>
       <c r="C312">
         <v>64</v>
@@ -7468,10 +7454,10 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
+        <v>189</v>
+      </c>
+      <c r="B313" t="s">
         <v>193</v>
-      </c>
-      <c r="B313" t="s">
-        <v>197</v>
       </c>
       <c r="C313">
         <v>128</v>
@@ -7482,10 +7468,10 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
+        <v>189</v>
+      </c>
+      <c r="B314" t="s">
         <v>193</v>
-      </c>
-      <c r="B314" t="s">
-        <v>197</v>
       </c>
       <c r="C314">
         <v>196</v>
@@ -7496,10 +7482,10 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
+        <v>189</v>
+      </c>
+      <c r="B315" t="s">
         <v>193</v>
-      </c>
-      <c r="B315" t="s">
-        <v>197</v>
       </c>
       <c r="C315">
         <v>256</v>
@@ -7510,7 +7496,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B316" t="s">
         <v>125</v>
@@ -7524,7 +7510,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B317" t="s">
         <v>125</v>
@@ -7538,7 +7524,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B318" t="s">
         <v>125</v>
@@ -7552,7 +7538,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B319" t="s">
         <v>125</v>
@@ -7566,7 +7552,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B320" t="s">
         <v>125</v>
@@ -7580,7 +7566,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B321" t="s">
         <v>125</v>
@@ -7594,7 +7580,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B322" t="s">
         <v>125</v>
@@ -7608,7 +7594,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B323" t="s">
         <v>125</v>
@@ -7622,7 +7608,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B324" t="s">
         <v>125</v>
@@ -7636,7 +7622,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B326" t="s">
         <v>131</v>
@@ -7650,7 +7636,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B327" t="s">
         <v>131</v>
@@ -7664,7 +7650,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B328" t="s">
         <v>132</v>
@@ -7678,7 +7664,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B329" t="s">
         <v>132</v>
@@ -7818,15 +7804,15 @@
         <v>49</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B346" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C346">
         <v>64</v>
@@ -7840,10 +7826,10 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B347" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C347">
         <v>128</v>
@@ -7857,10 +7843,10 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B348" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C348">
         <v>196</v>
@@ -7874,10 +7860,10 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B349" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C349">
         <v>256</v>
@@ -7891,10 +7877,10 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B350" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C350">
         <v>384</v>
@@ -7908,10 +7894,10 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B351" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C351">
         <v>512</v>
@@ -7925,10 +7911,10 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B352" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C352">
         <v>768</v>
@@ -7942,10 +7928,10 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B353" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C353">
         <v>1000</v>
@@ -7959,10 +7945,10 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B354" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C354">
         <v>1500</v>
@@ -7993,12 +7979,12 @@
         <v>49</v>
       </c>
       <c r="E357" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B358" t="s">
         <v>128</v>
@@ -8015,7 +8001,7 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B359" t="s">
         <v>128</v>
@@ -8032,7 +8018,7 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B360" t="s">
         <v>128</v>
@@ -8049,7 +8035,7 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B362" t="s">
         <v>128</v>
@@ -8066,7 +8052,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B363" t="s">
         <v>128</v>
@@ -8083,7 +8069,7 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B364" t="s">
         <v>128</v>
@@ -8614,7 +8600,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>43</v>
@@ -8668,7 +8654,7 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -8706,10 +8692,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0BE0C2-6CFA-B544-AD1B-E0CD7C820A66}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8741,7 +8727,7 @@
       <c r="B4" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>100</v>
       </c>
     </row>
@@ -8763,7 +8749,7 @@
       <c r="B6" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>100</v>
       </c>
     </row>
@@ -8775,50 +8761,6 @@
         <v>170</v>
       </c>
       <c r="C7" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" t="s">
-        <v>170</v>
-      </c>
-      <c r="C10" s="16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="12">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates supporting integration of PCAP feeds
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/embedded.xlsx
+++ b/xlsxPCES/examples/embedded.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld/xlsxPCES/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4379B6-9954-3947-A706-224B7B310D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9BF594-12FE-164C-AB02-CD0A79CFD320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="840" windowWidth="34560" windowHeight="20160" activeTab="5" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="0" yWindow="1380" windowWidth="34200" windowHeight="19640" activeTab="1" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
-    <sheet name="cp" sheetId="3" r:id="rId2"/>
-    <sheet name="execTime" sheetId="4" r:id="rId3"/>
-    <sheet name="mapping" sheetId="2" r:id="rId4"/>
-    <sheet name="netParams" sheetId="5" r:id="rId5"/>
-    <sheet name="experiments" sheetId="6" r:id="rId6"/>
+    <sheet name="ipmap" sheetId="7" r:id="rId2"/>
+    <sheet name="cp" sheetId="3" r:id="rId3"/>
+    <sheet name="execTime" sheetId="4" r:id="rId4"/>
+    <sheet name="mapping" sheetId="2" r:id="rId5"/>
+    <sheet name="netParams" sheetId="5" r:id="rId6"/>
+    <sheet name="experiments" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="233">
   <si>
     <t>Networks</t>
   </si>
@@ -656,6 +657,87 @@
   </si>
   <si>
     <t>exec time (usec)</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>internal IP</t>
+  </si>
+  <si>
+    <t>external IP</t>
+  </si>
+  <si>
+    <t>10.0.1.1</t>
+  </si>
+  <si>
+    <t>10.0.1.2</t>
+  </si>
+  <si>
+    <t>10.0.1.3</t>
+  </si>
+  <si>
+    <t>internal CIDR</t>
+  </si>
+  <si>
+    <t>external  CIDR</t>
+  </si>
+  <si>
+    <t>10.0.1.0/24</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>dilation factor</t>
+  </si>
+  <si>
+    <t>first arrival (sec)</t>
+  </si>
+  <si>
+    <t>/tmp/pces.sock</t>
+  </si>
+  <si>
+    <t>192.168.66.33</t>
+  </si>
+  <si>
+    <t>192.168.66.34</t>
+  </si>
+  <si>
+    <t>192.168.66.0/24</t>
+  </si>
+  <si>
+    <t>Feed1</t>
+  </si>
+  <si>
+    <t>time (clock, packet)</t>
+  </si>
+  <si>
+    <t>packet</t>
+  </si>
+  <si>
+    <t>src type (file, unix-socket, net-socket)</t>
+  </si>
+  <si>
+    <t>src spec (file name or port number)</t>
+  </si>
+  <si>
+    <t>Feed IP</t>
+  </si>
+  <si>
+    <t>10.0.1.1:8881</t>
+  </si>
+  <si>
+    <t>### feed class</t>
+  </si>
+  <si>
+    <t>feed</t>
+  </si>
+  <si>
+    <t>unix-socket</t>
   </si>
 </sst>
 </file>
@@ -665,7 +747,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -812,6 +894,12 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1238,7 +1326,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1263,6 +1351,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1640,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95325CDA-052A-9A47-A8FD-348C19C2091E}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1977,11 +2068,234 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EA2AF0-37BC-7041-B363-E1C87D90F910}">
+  <dimension ref="A2:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2.33</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA9935-1338-5743-9994-8B53C9940146}">
-  <dimension ref="A3:M100"/>
+  <dimension ref="A3:M105"/>
   <sheetViews>
-    <sheetView topLeftCell="E42" zoomScale="155" zoomScaleNormal="164" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView topLeftCell="A55" zoomScale="155" zoomScaleNormal="164" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1989,7 +2303,7 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="8" width="21.6640625" customWidth="1"/>
@@ -2663,7 +2977,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>85</v>
       </c>
@@ -2692,7 +3006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -2712,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -2732,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>99</v>
       </c>
@@ -2764,35 +3078,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B72" t="s">
-        <v>101</v>
-      </c>
-      <c r="C72" t="s">
-        <v>102</v>
-      </c>
-      <c r="D72">
-        <v>1000</v>
-      </c>
-      <c r="E72">
-        <v>1500</v>
-      </c>
-      <c r="F72" t="s">
-        <v>30</v>
-      </c>
-      <c r="G72">
-        <v>10</v>
-      </c>
-      <c r="I72" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>86</v>
+        <v>230</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>142</v>
@@ -2801,76 +3089,41 @@
         <v>143</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="B75" t="s">
         <v>101</v>
       </c>
       <c r="C75" t="s">
-        <v>72</v>
-      </c>
-      <c r="D75" t="b">
+        <v>102</v>
+      </c>
+      <c r="D75" t="s">
+        <v>229</v>
+      </c>
+      <c r="G75" t="b">
         <v>0</v>
       </c>
-      <c r="E75" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>142</v>
@@ -2878,196 +3131,274 @@
       <c r="C79" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>150</v>
+      <c r="D79" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G79" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H79" s="5" t="s">
+      <c r="F79" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="K79" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="L79" s="4" t="s">
+      <c r="G79" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H79" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B80" t="s">
         <v>101</v>
       </c>
       <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K84" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="L84" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>33</v>
+      </c>
+      <c r="B85" t="s">
+        <v>101</v>
+      </c>
+      <c r="C85" t="s">
         <v>105</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D85" t="s">
         <v>113</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E85" t="s">
         <v>125</v>
       </c>
-      <c r="F80" t="b">
+      <c r="F85" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>33</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B87" t="s">
         <v>101</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C87" t="s">
         <v>160</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D87" t="s">
         <v>20</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E87" t="s">
         <v>200</v>
       </c>
-      <c r="F82" t="b">
+      <c r="F87" t="b">
         <v>1</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I87" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>33</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B89" t="s">
         <v>101</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C89" t="s">
         <v>161</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D89" t="s">
         <v>117</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E89" t="s">
         <v>199</v>
       </c>
-      <c r="F84" t="b">
+      <c r="F89" t="b">
         <v>1</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I89" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>33</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B91" t="s">
         <v>101</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C91" t="s">
         <v>106</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D91" t="s">
         <v>118</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E91" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>33</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B93" t="s">
         <v>108</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D93" t="s">
         <v>118</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E93" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="G97" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="H92" s="1" t="s">
+      <c r="H97" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I92" s="5" t="s">
+      <c r="I97" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="J92" s="5" t="s">
+      <c r="J97" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="K92" s="4" t="s">
+      <c r="K97" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+    <row r="102" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
+    <row r="103" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3076,11 +3407,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E788907-EF7B-7245-8B51-85EEFFE3B34D}">
   <dimension ref="A1:E374"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A360" zoomScale="150" workbookViewId="0">
       <selection activeCell="E286" sqref="E286"/>
     </sheetView>
   </sheetViews>
@@ -8165,7 +8496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CD1F53-6FA9-024B-AEB4-78F83AE23C0B}">
   <dimension ref="A3:D31"/>
   <sheetViews>
@@ -8455,7 +8786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04436424-07DF-B343-BAAE-706A3CFD4756}">
   <dimension ref="A2:K24"/>
   <sheetViews>
@@ -8690,12 +9021,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0BE0C2-6CFA-B544-AD1B-E0CD7C820A66}">
   <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="150" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>